<commit_message>
dev-1.1.0 : export trace-list
</commit_message>
<xml_diff>
--- a/storage/template/xl_barcode.xlsx
+++ b/storage/template/xl_barcode.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\avicennaa\storage\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp5\htdocs\avicenna\storage\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="4470"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7476" windowHeight="4476"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,18 +24,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>TRACEBILITY DEMO</t>
   </si>
   <si>
-    <t>15011417A06C005</t>
-  </si>
-  <si>
     <t>PART NUMBER</t>
-  </si>
-  <si>
-    <t>OIL PAN</t>
   </si>
   <si>
     <t>PART MODEL</t>
@@ -43,18 +37,12 @@
   <si>
     <t>PART CODE</t>
   </si>
-  <si>
-    <t>TES</t>
-  </si>
-  <si>
-    <t>*15011417A06C005*</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -408,12 +396,12 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E8"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="21">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -422,100 +410,90 @@
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>7</v>
-      </c>
+    <row r="2" spans="1:5">
+      <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B9" s="1"/>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="B10" s="1"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="B11" s="1"/>
-      <c r="C11" s="4" t="s">
-        <v>6</v>
-      </c>
+      <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>3</v>
-      </c>
+    <row r="12" spans="1:5">
+      <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>

</xml_diff>

<commit_message>
dev-1.1.0 : edit excel download barcode traceability manual
</commit_message>
<xml_diff>
--- a/storage/template/xl_barcode.xlsx
+++ b/storage/template/xl_barcode.xlsx
@@ -26,21 +26,12 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
-    <t>TRACEBILITY DEMO</t>
-  </si>
-  <si>
     <t>15011417A06C005</t>
   </si>
   <si>
-    <t>PART NUMBER</t>
-  </si>
-  <si>
     <t>OIL PAN</t>
   </si>
   <si>
-    <t>PART MODEL</t>
-  </si>
-  <si>
     <t>PART CODE</t>
   </si>
   <si>
@@ -48,13 +39,22 @@
   </si>
   <si>
     <t>*15011417A06C005*</t>
+  </si>
+  <si>
+    <t>PART NUMBER AIIA</t>
+  </si>
+  <si>
+    <t>PART MODEL AIIA</t>
+  </si>
+  <si>
+    <t>TRACEBILITY</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -408,114 +408,114 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E8"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="21">
       <c r="A1" s="2" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10" s="1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="4" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="4" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12" s="5" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>

</xml_diff>